<commit_message>
Base for a procedural commentor to day 21
</commit_message>
<xml_diff>
--- a/day21/Prepsheet.xlsx
+++ b/day21/Prepsheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lars-\source\repos\private\aoc\2021\day21\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BA6097B0-44D8-4106-88E0-415A008E54D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D2C86F7-6ED1-4DE8-AFC5-39E52B0326EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21390" activeTab="2" xr2:uid="{C608AD6E-4B7C-4DA4-8A47-1467F5E32675}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" activeTab="2" xr2:uid="{C608AD6E-4B7C-4DA4-8A47-1467F5E32675}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -4503,10 +4503,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7028F918-4490-494F-B795-383B49BEF384}">
-  <dimension ref="B2:J35"/>
+  <dimension ref="B2:P35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+      <selection activeCell="P19" sqref="P19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4514,9 +4514,13 @@
     <col min="2" max="2" width="25.42578125" customWidth="1"/>
     <col min="4" max="4" width="19.42578125" style="6" customWidth="1"/>
     <col min="5" max="5" width="3" style="6" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.7109375" customWidth="1"/>
+    <col min="16" max="16" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B2" s="6">
         <v>444356092776315</v>
       </c>
@@ -4535,7 +4539,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B3" s="6">
         <v>341960390180808</v>
       </c>
@@ -4555,7 +4559,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B4" s="6">
         <f>B2+B3</f>
         <v>786316482957123</v>
@@ -4576,7 +4580,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B5" t="str">
         <f>TEXT(B4,"0")</f>
         <v>786316482957123</v>
@@ -4597,7 +4601,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B6">
         <f>LEN(B5)</f>
         <v>15</v>
@@ -4618,7 +4622,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:16" x14ac:dyDescent="0.25">
       <c r="D7" s="6">
         <f t="shared" si="2"/>
         <v>729</v>
@@ -4635,7 +4639,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:16" x14ac:dyDescent="0.25">
       <c r="D8" s="6">
         <f t="shared" si="2"/>
         <v>2187</v>
@@ -4652,7 +4656,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:16" x14ac:dyDescent="0.25">
       <c r="D9" s="6">
         <f t="shared" si="2"/>
         <v>6561</v>
@@ -4669,7 +4673,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:16" x14ac:dyDescent="0.25">
       <c r="D10" s="6">
         <f t="shared" si="2"/>
         <v>19683</v>
@@ -4686,7 +4690,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:16" x14ac:dyDescent="0.25">
       <c r="D11" s="6">
         <f t="shared" si="2"/>
         <v>59049</v>
@@ -4703,7 +4707,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:16" x14ac:dyDescent="0.25">
       <c r="D12" s="6">
         <f t="shared" si="2"/>
         <v>177147</v>
@@ -4720,7 +4724,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:16" x14ac:dyDescent="0.25">
       <c r="D13" s="6">
         <f t="shared" si="2"/>
         <v>531441</v>
@@ -4737,7 +4741,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:16" x14ac:dyDescent="0.25">
       <c r="D14" s="6">
         <f t="shared" si="2"/>
         <v>1594323</v>
@@ -4755,7 +4759,7 @@
       </c>
       <c r="J14" s="6"/>
     </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:16" x14ac:dyDescent="0.25">
       <c r="D15" s="6">
         <f>D14*3</f>
         <v>4782969</v>
@@ -4772,7 +4776,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:16" x14ac:dyDescent="0.25">
       <c r="D16" s="6">
         <f t="shared" si="2"/>
         <v>14348907</v>
@@ -4789,11 +4793,27 @@
         <v>5</v>
       </c>
       <c r="I16" s="6">
-        <f>D13+3359232</f>
-        <v>3890673</v>
-      </c>
-    </row>
-    <row r="17" spans="4:7" x14ac:dyDescent="0.25">
+        <v>14348907</v>
+      </c>
+      <c r="J16">
+        <v>3359232</v>
+      </c>
+      <c r="K16">
+        <f>J16*27</f>
+        <v>90699264</v>
+      </c>
+      <c r="N16">
+        <v>10989675</v>
+      </c>
+      <c r="O16">
+        <v>3359232</v>
+      </c>
+      <c r="P16">
+        <f>N16+O16</f>
+        <v>14348907</v>
+      </c>
+    </row>
+    <row r="17" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D17" s="6">
         <f t="shared" si="2"/>
         <v>43046721</v>
@@ -4810,7 +4830,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D18" s="6">
         <f t="shared" si="2"/>
         <v>129140163</v>
@@ -4827,7 +4847,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D19" s="6">
         <f t="shared" si="2"/>
         <v>387420489</v>
@@ -4843,8 +4863,30 @@
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="20" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="I19">
+        <v>300080457</v>
+      </c>
+      <c r="J19" s="6"/>
+      <c r="K19">
+        <f>I19+K16</f>
+        <v>390779721</v>
+      </c>
+      <c r="L19" s="6">
+        <f>K19-D19</f>
+        <v>3359232</v>
+      </c>
+      <c r="N19">
+        <v>270641475</v>
+      </c>
+      <c r="O19">
+        <v>29438982</v>
+      </c>
+      <c r="P19">
+        <f>N19+O19</f>
+        <v>300080457</v>
+      </c>
+    </row>
+    <row r="20" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D20" s="6">
         <f t="shared" si="2"/>
         <v>1162261467</v>
@@ -4861,7 +4903,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D21" s="6">
         <f t="shared" si="2"/>
         <v>3486784401</v>
@@ -4878,7 +4920,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="22" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D22" s="6">
         <f t="shared" si="2"/>
         <v>10460353203</v>
@@ -4895,7 +4937,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="23" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D23" s="6">
         <f t="shared" si="2"/>
         <v>31381059609</v>
@@ -4912,7 +4954,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="24" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D24" s="6">
         <f t="shared" si="2"/>
         <v>94143178827</v>
@@ -4929,7 +4971,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="25" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D25" s="6">
         <f t="shared" ref="D25:D31" si="3">D24*3</f>
         <v>282429536481</v>
@@ -4946,7 +4988,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="26" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D26" s="6">
         <f t="shared" si="3"/>
         <v>847288609443</v>
@@ -4963,7 +5005,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="27" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D27" s="6">
         <f t="shared" si="3"/>
         <v>2541865828329</v>
@@ -4980,7 +5022,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="28" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D28" s="6">
         <f t="shared" si="3"/>
         <v>7625597484987</v>
@@ -4997,7 +5039,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="29" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D29" s="6">
         <f t="shared" si="3"/>
         <v>22876792454961</v>
@@ -5014,7 +5056,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="30" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D30" s="6">
         <f t="shared" si="3"/>
         <v>68630377364883</v>
@@ -5031,7 +5073,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="31" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D31" s="6">
         <f t="shared" si="3"/>
         <v>205891132094649</v>
@@ -5048,7 +5090,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="32" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D32" s="6">
         <f t="shared" ref="D32:D35" si="4">D31*3</f>
         <v>617673396283947</v>

</xml_diff>